<commit_message>
did the second and thrid task(show memeber pofile and create a member profile)
</commit_message>
<xml_diff>
--- a/Sprint_Backlog_Template.xlsx
+++ b/Sprint_Backlog_Template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SE\Hello-World\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576D74AB-4508-4BC5-A987-1B62F8701FF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,7 +243,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,7 +352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,26 +385,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,23 +420,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -635,21 +595,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="82.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="82.5703125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -675,7 +635,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -688,8 +648,11 @@
       <c r="D2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -702,8 +665,11 @@
       <c r="D3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -716,8 +682,11 @@
       <c r="D4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.3</v>
       </c>
@@ -731,7 +700,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -745,7 +714,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1.5</v>
       </c>
@@ -759,7 +728,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1.6</v>
       </c>
@@ -776,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1.7</v>
       </c>
@@ -793,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1.8</v>
       </c>
@@ -810,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1.9</v>
       </c>
@@ -827,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -844,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2.1</v>
       </c>
@@ -861,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2.2000000000000002</v>
       </c>
@@ -878,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2.2999999999999998</v>
       </c>
@@ -895,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2.4</v>
       </c>
@@ -912,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2.5</v>
       </c>
@@ -929,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2.6</v>
       </c>
@@ -946,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2.7</v>
       </c>
@@ -963,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2.8</v>
       </c>
@@ -980,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2.9</v>
       </c>
@@ -997,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1014,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3.1</v>
       </c>
@@ -1028,7 +997,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -1042,7 +1011,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3.3</v>
       </c>
@@ -1062,7 +1031,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3.4</v>
       </c>
@@ -1076,7 +1045,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3.5</v>
       </c>
@@ -1096,7 +1065,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3.6</v>
       </c>
@@ -1116,7 +1085,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3.7</v>
       </c>
@@ -1130,7 +1099,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3.8</v>
       </c>
@@ -1147,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3.9</v>
       </c>
@@ -1167,7 +1136,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1184,7 +1153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4.0999999999999996</v>
       </c>
@@ -1198,7 +1167,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4.2</v>
       </c>
@@ -1212,7 +1181,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4.3</v>
       </c>
@@ -1226,7 +1195,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4.4000000000000004</v>
       </c>
@@ -1240,7 +1209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4.5</v>
       </c>
@@ -1257,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4.5999999999999996</v>
       </c>
@@ -1274,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4.7</v>
       </c>
@@ -1288,7 +1257,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4.8</v>
       </c>
@@ -1302,7 +1271,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4.9000000000000004</v>
       </c>
@@ -1316,7 +1285,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1330,7 +1299,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>5.0999999999999996</v>
       </c>
@@ -1344,7 +1313,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5.2</v>
       </c>
@@ -1358,7 +1327,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>5.3</v>
       </c>
@@ -1372,7 +1341,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5.4</v>
       </c>
@@ -1386,7 +1355,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>5.5</v>
       </c>
@@ -1400,7 +1369,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>5.6</v>
       </c>
@@ -1414,7 +1383,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>5.7</v>
       </c>
@@ -1434,7 +1403,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5.8</v>
       </c>
@@ -1448,7 +1417,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5.9</v>
       </c>
@@ -1462,7 +1431,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1476,7 +1445,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>6.1</v>
       </c>
@@ -1490,7 +1459,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>6.2</v>
       </c>
@@ -1504,7 +1473,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>6.3</v>
       </c>
@@ -1518,7 +1487,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>6.4</v>
       </c>
@@ -1532,7 +1501,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>6.5</v>
       </c>
@@ -1546,7 +1515,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>6.6</v>
       </c>
@@ -1574,24 +1543,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
did the 4th,5th and the 6th tasks but i cant test for some reason
</commit_message>
<xml_diff>
--- a/Sprint_Backlog_Template.xlsx
+++ b/Sprint_Backlog_Template.xlsx
@@ -599,7 +599,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,6 +699,9 @@
       <c r="D5" t="s">
         <v>61</v>
       </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -713,6 +716,9 @@
       <c r="D6" t="s">
         <v>61</v>
       </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -727,6 +733,9 @@
       <c r="D7" t="s">
         <v>61</v>
       </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1383,7 +1392,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5.7</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5.8</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.9</v>
       </c>
@@ -1431,7 +1440,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6.1</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>6.2</v>
       </c>
@@ -1473,7 +1482,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>6.3</v>
       </c>
@@ -1487,7 +1496,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>6.4</v>
       </c>
@@ -1501,7 +1510,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>6.5</v>
       </c>
@@ -1515,7 +1524,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6.6</v>
       </c>

</xml_diff>

<commit_message>
Updated Sprint Backlog and Added Sprint 1 Report
</commit_message>
<xml_diff>
--- a/Sprint_Backlog_Template.xlsx
+++ b/Sprint_Backlog_Template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SE\Hello-World\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46995501-DBCD-49A9-A26A-15367D9E5807}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>User story</t>
   </si>
@@ -237,13 +243,61 @@
     <t>Test Integration</t>
   </si>
   <si>
-    <t>DONE</t>
+    <t>A Member should be able to add skills to his profile</t>
+  </si>
+  <si>
+    <t>A Member Should be able to add certificates to his profile</t>
+  </si>
+  <si>
+    <t>A Member Should  be able to add completed tasks to his profile</t>
+  </si>
+  <si>
+    <t>A Member Should be able to add interests to his profile</t>
+  </si>
+  <si>
+    <t>A Member Should be able to add Past Events to his Profile</t>
+  </si>
+  <si>
+    <t>A Partner Should be able to add Board Members to his profile</t>
+  </si>
+  <si>
+    <t>A Partner Should be able to add Partners to his profile</t>
+  </si>
+  <si>
+    <t>A Partneer Should be able to add events to his profile</t>
+  </si>
+  <si>
+    <t>A Partner Should be able to add project to his past projects</t>
+  </si>
+  <si>
+    <t>A Consultant Should be able Board Members to his Profile</t>
+  </si>
+  <si>
+    <t>A Consultant Should be able to add Partners to his profile</t>
+  </si>
+  <si>
+    <t>A Consultant Should be able to add reports to his profile</t>
+  </si>
+  <si>
+    <t>A Consultant Should be able to add events to his Profile</t>
+  </si>
+  <si>
+    <t>An Educational Organization Should be able to add Courses to their Profile</t>
+  </si>
+  <si>
+    <t>An Educational Organization Should be able to add Trainers to their Profile</t>
+  </si>
+  <si>
+    <t>An Educational Organization Should be able to add Certificates to their Profile</t>
+  </si>
+  <si>
+    <t>An Educational Organization Should be able to add Training Programs to their Profile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,7 +406,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,9 +439,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,6 +491,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -595,21 +683,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="82.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="82.5546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -631,11 +719,9 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -648,11 +734,8 @@
       <c r="D2" t="s">
         <v>61</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -665,11 +748,8 @@
       <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -682,11 +762,8 @@
       <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.3</v>
       </c>
@@ -699,11 +776,8 @@
       <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -716,11 +790,8 @@
       <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1.5</v>
       </c>
@@ -733,11 +804,8 @@
       <c r="D7" t="s">
         <v>61</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1.6</v>
       </c>
@@ -750,11 +818,8 @@
       <c r="D8" t="s">
         <v>63</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1.7</v>
       </c>
@@ -767,11 +832,8 @@
       <c r="D9" t="s">
         <v>63</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1.8</v>
       </c>
@@ -784,11 +846,8 @@
       <c r="D10" t="s">
         <v>63</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1.9</v>
       </c>
@@ -801,11 +860,8 @@
       <c r="D11" t="s">
         <v>63</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -818,11 +874,8 @@
       <c r="D12" t="s">
         <v>63</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2.1</v>
       </c>
@@ -835,11 +888,8 @@
       <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2.2000000000000002</v>
       </c>
@@ -852,11 +902,8 @@
       <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2.2999999999999998</v>
       </c>
@@ -869,11 +916,8 @@
       <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2.4</v>
       </c>
@@ -886,11 +930,8 @@
       <c r="D16" t="s">
         <v>62</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2.5</v>
       </c>
@@ -903,11 +944,8 @@
       <c r="D17" t="s">
         <v>62</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2.6</v>
       </c>
@@ -920,11 +958,8 @@
       <c r="D18" t="s">
         <v>60</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2.7</v>
       </c>
@@ -937,11 +972,8 @@
       <c r="D19" t="s">
         <v>60</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2.8</v>
       </c>
@@ -954,11 +986,8 @@
       <c r="D20" t="s">
         <v>60</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2.9</v>
       </c>
@@ -971,11 +1000,8 @@
       <c r="D21" t="s">
         <v>60</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -988,11 +1014,8 @@
       <c r="D22" t="s">
         <v>60</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3.1</v>
       </c>
@@ -1006,7 +1029,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -1020,7 +1043,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3.3</v>
       </c>
@@ -1040,7 +1063,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3.4</v>
       </c>
@@ -1054,7 +1077,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3.5</v>
       </c>
@@ -1074,7 +1097,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3.6</v>
       </c>
@@ -1094,7 +1117,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3.7</v>
       </c>
@@ -1108,7 +1131,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3.8</v>
       </c>
@@ -1121,11 +1144,8 @@
       <c r="D30" t="s">
         <v>58</v>
       </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3.9</v>
       </c>
@@ -1145,7 +1165,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1158,11 +1178,8 @@
       <c r="D32" t="s">
         <v>58</v>
       </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4.0999999999999996</v>
       </c>
@@ -1176,7 +1193,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4.2</v>
       </c>
@@ -1190,7 +1207,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4.3</v>
       </c>
@@ -1204,7 +1221,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4.4000000000000004</v>
       </c>
@@ -1218,7 +1235,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4.5</v>
       </c>
@@ -1231,11 +1248,8 @@
       <c r="D37" t="s">
         <v>55</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4.5999999999999996</v>
       </c>
@@ -1248,11 +1262,8 @@
       <c r="D38" t="s">
         <v>55</v>
       </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4.7</v>
       </c>
@@ -1266,7 +1277,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4.8</v>
       </c>
@@ -1280,7 +1291,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4.9000000000000004</v>
       </c>
@@ -1294,7 +1305,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1308,7 +1319,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>5.0999999999999996</v>
       </c>
@@ -1322,7 +1333,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5.2</v>
       </c>
@@ -1336,7 +1347,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>5.3</v>
       </c>
@@ -1350,7 +1361,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5.4</v>
       </c>
@@ -1364,7 +1375,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>5.5</v>
       </c>
@@ -1378,7 +1389,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>5.6</v>
       </c>
@@ -1392,7 +1403,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>5.7</v>
       </c>
@@ -1412,7 +1423,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5.8</v>
       </c>
@@ -1426,7 +1437,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5.9</v>
       </c>
@@ -1440,7 +1451,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1454,7 +1465,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>6.1</v>
       </c>
@@ -1468,7 +1479,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>6.2</v>
       </c>
@@ -1482,7 +1493,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>6.3</v>
       </c>
@@ -1496,7 +1507,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>6.4</v>
       </c>
@@ -1510,7 +1521,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>6.5</v>
       </c>
@@ -1524,7 +1535,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>6.6</v>
       </c>
@@ -1536,6 +1547,244 @@
       </c>
       <c r="D58" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>6.7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>6.8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>6.9</v>
+      </c>
+      <c r="B61" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>7.1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>7.2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>7.3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>7.4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>7.5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>7.6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>7.7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>7.8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>7.9</v>
+      </c>
+      <c r="B71" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>8</v>
+      </c>
+      <c r="B72" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>8.1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B74" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B75" t="s">
+        <v>89</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1552,24 +1801,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>